<commit_message>
Update Data_Dictionary - Updated Dec 2020 V3.xlsx
Updated definitions
</commit_message>
<xml_diff>
--- a/Data_Dictionary - Updated Dec 2020 V3.xlsx
+++ b/Data_Dictionary - Updated Dec 2020 V3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mary.amanuel/Documents/My Tableau Repository/Datasources/2020.1/en_GB-EU/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arouba.zubair/Documents/GitHub/NHS-App-Analytics-Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B069A41-5096-E24A-9E1D-BC9E1F73C403}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E29500-93C0-E349-8B6C-56B4800FCD8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="28800" windowHeight="16520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,6 +77,7 @@
         <sz val="11"/>
         <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>Denominator: NHS Digital (published)</t>
     </r>
@@ -139,13 +140,7 @@
     <t>Users Booking Appointments</t>
   </si>
   <si>
-    <t>Number of App users booking GP Practice Appointments in the specified reporting period</t>
-  </si>
-  <si>
     <t>Appointment Cancellation</t>
-  </si>
-  <si>
-    <t>Number of appointment cancelled from the NHS App in the specified reporting period</t>
   </si>
   <si>
     <t>Users Requesting Prescriptions</t>
@@ -511,6 +506,12 @@
   <si>
     <t>Data is restricted to those practices that have consented to share data and are list on the GP Workload Participation List.</t>
   </si>
+  <si>
+    <t>Number of App users cancelling GP appointments in the specified reporting period</t>
+  </si>
+  <si>
+    <t>Number of App users booking GP appointments in the specified reporting period</t>
+  </si>
 </sst>
 </file>
 
@@ -527,74 +528,87 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -834,11 +848,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1060,7 +1074,7 @@
   </sheetPr>
   <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="160" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1121,7 +1135,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="8" t="s">
@@ -1161,7 +1175,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -1176,10 +1190,10 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
@@ -1194,10 +1208,10 @@
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
@@ -1217,7 +1231,7 @@
         <v>28</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
@@ -1236,12 +1250,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>32</v>
+        <v>154</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>8</v>
@@ -1254,10 +1268,10 @@
     </row>
     <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>34</v>
+        <v>153</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>8</v>
@@ -1270,10 +1284,10 @@
     </row>
     <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>8</v>
@@ -1286,10 +1300,10 @@
     </row>
     <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>8</v>
@@ -1302,17 +1316,17 @@
     </row>
     <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>9</v>
@@ -1320,10 +1334,10 @@
     </row>
     <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>8</v>
@@ -1336,10 +1350,10 @@
     </row>
     <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>8</v>
@@ -1352,10 +1366,10 @@
     </row>
     <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>8</v>
@@ -1368,17 +1382,17 @@
     </row>
     <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>9</v>
@@ -1386,17 +1400,17 @@
     </row>
     <row r="19" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>9</v>
@@ -2233,7 +2247,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -2242,7 +2256,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>3</v>
@@ -2259,10 +2273,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>8</v>
@@ -2278,10 +2292,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>8</v>
@@ -2300,17 +2314,17 @@
         <v>10</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D4" s="28" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F4" s="28"/>
       <c r="G4" s="18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.15">
@@ -2330,7 +2344,7 @@
       <c r="E6" s="30"/>
       <c r="F6" s="30"/>
       <c r="G6" s="19" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H6" s="20"/>
     </row>
@@ -2342,14 +2356,14 @@
         <v>13</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G7" s="16"/>
     </row>
@@ -2369,7 +2383,7 @@
         <v>19</v>
       </c>
       <c r="G8" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="96" x14ac:dyDescent="0.15">
@@ -2380,13 +2394,13 @@
         <v>25</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>28</v>
@@ -2403,7 +2417,7 @@
         <v>20</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>8</v>
@@ -3456,7 +3470,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -3465,7 +3479,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>3</v>
@@ -3485,7 +3499,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>8</v>
@@ -3501,10 +3515,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -3518,10 +3532,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D4" s="16" t="s">
         <v>8</v>
@@ -3537,10 +3551,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>8</v>
@@ -3554,18 +3568,18 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.15">
@@ -3576,7 +3590,7 @@
         <v>29</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>8</v>
@@ -3592,10 +3606,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>8</v>
@@ -3609,10 +3623,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>8</v>
@@ -3628,10 +3642,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>8</v>
@@ -3647,10 +3661,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>8</v>
@@ -3666,10 +3680,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D12" s="16" t="s">
         <v>8</v>
@@ -3685,17 +3699,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G13" s="16" t="s">
         <v>9</v>
@@ -3706,10 +3720,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D14" s="16" t="s">
         <v>8</v>
@@ -3725,10 +3739,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>8</v>
@@ -3742,10 +3756,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>8</v>
@@ -3761,10 +3775,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C17" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>8</v>
@@ -3778,10 +3792,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>8</v>
@@ -3797,10 +3811,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>8</v>
@@ -3814,17 +3828,17 @@
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C20" s="16" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D20" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G20" s="16" t="s">
         <v>9</v>
@@ -3835,17 +3849,17 @@
         <v>20</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D21" s="16" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="16"/>
       <c r="F21" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G21" s="16" t="s">
         <v>9</v>
@@ -4856,7 +4870,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.15">
       <c r="A1" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -4865,7 +4879,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>3</v>
@@ -4885,7 +4899,7 @@
         <v>6</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D2" s="16" t="s">
         <v>8</v>
@@ -4901,18 +4915,18 @@
         <v>2</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D3" s="28"/>
       <c r="E3" s="28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F3" s="32"/>
       <c r="G3" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.15">
@@ -4923,7 +4937,7 @@
       <c r="E4" s="30"/>
       <c r="F4" s="33"/>
       <c r="G4" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.15">
@@ -4931,10 +4945,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5" s="16"/>
       <c r="E5" s="16"/>
@@ -4946,14 +4960,14 @@
     <row r="6" spans="1:7" ht="64" x14ac:dyDescent="0.15">
       <c r="A6" s="14"/>
       <c r="B6" s="15" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
@@ -4963,10 +4977,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>8</v>
@@ -4982,10 +4996,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D8" s="16" t="s">
         <v>8</v>
@@ -4999,18 +5013,18 @@
         <v>6</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D9" s="16"/>
       <c r="E9" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.15">
@@ -5021,7 +5035,7 @@
         <v>29</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" s="16" t="s">
         <v>8</v>
@@ -5037,18 +5051,18 @@
         <v>8</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F11" s="32"/>
       <c r="G11" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.15">
@@ -5059,7 +5073,7 @@
       <c r="E12" s="30"/>
       <c r="F12" s="33"/>
       <c r="G12" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="32" x14ac:dyDescent="0.15">
@@ -5067,10 +5081,10 @@
         <v>9</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>8</v>
@@ -5084,18 +5098,18 @@
         <v>10</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.15">
@@ -5106,7 +5120,7 @@
       <c r="E15" s="30"/>
       <c r="F15" s="33"/>
       <c r="G15" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="48" x14ac:dyDescent="0.15">
@@ -5114,10 +5128,10 @@
         <v>11</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>8</v>
@@ -5133,18 +5147,18 @@
         <v>12</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C17" s="28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D17" s="28"/>
       <c r="E17" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F17" s="32"/>
       <c r="G17" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.15">
@@ -5155,7 +5169,7 @@
       <c r="E18" s="30"/>
       <c r="F18" s="33"/>
       <c r="G18" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="32" x14ac:dyDescent="0.15">
@@ -5163,10 +5177,10 @@
         <v>13</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D19" s="16" t="s">
         <v>8</v>
@@ -5182,18 +5196,18 @@
         <v>14</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="28" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F20" s="32"/>
       <c r="G20" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5204,7 +5218,7 @@
       <c r="E21" s="30"/>
       <c r="F21" s="33"/>
       <c r="G21" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5212,10 +5226,10 @@
         <v>15</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>8</v>
@@ -5231,18 +5245,18 @@
         <v>16</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D23" s="28"/>
       <c r="E23" s="28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5253,7 +5267,7 @@
       <c r="E24" s="30"/>
       <c r="F24" s="33"/>
       <c r="G24" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5261,10 +5275,10 @@
         <v>17</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D25" s="16" t="s">
         <v>8</v>
@@ -5280,18 +5294,18 @@
         <v>18</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D26" s="28"/>
       <c r="E26" s="28" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5302,7 +5316,7 @@
       <c r="E27" s="30"/>
       <c r="F27" s="33"/>
       <c r="G27" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5310,10 +5324,10 @@
         <v>19</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D28" s="16" t="s">
         <v>8</v>
@@ -5329,10 +5343,10 @@
         <v>20</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D29" s="16" t="s">
         <v>8</v>
@@ -5346,18 +5360,18 @@
         <v>21</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C30" s="28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D30" s="28"/>
       <c r="E30" s="28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F30" s="32"/>
       <c r="G30" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5368,7 +5382,7 @@
       <c r="E31" s="30"/>
       <c r="F31" s="33"/>
       <c r="G31" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5376,10 +5390,10 @@
         <v>22</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D32" s="16" t="s">
         <v>8</v>
@@ -5395,10 +5409,10 @@
         <v>23</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D33" s="16" t="s">
         <v>8</v>
@@ -5412,18 +5426,18 @@
         <v>24</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C34" s="28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D34" s="28"/>
       <c r="E34" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F34" s="32"/>
       <c r="G34" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5434,7 +5448,7 @@
       <c r="E35" s="30"/>
       <c r="F35" s="33"/>
       <c r="G35" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5442,10 +5456,10 @@
         <v>25</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C36" s="16" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D36" s="16" t="s">
         <v>8</v>
@@ -5461,10 +5475,10 @@
         <v>26</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D37" s="16" t="s">
         <v>8</v>
@@ -5478,18 +5492,18 @@
         <v>27</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D38" s="28"/>
       <c r="E38" s="28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F38" s="32"/>
       <c r="G38" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -5500,7 +5514,7 @@
       <c r="E39" s="30"/>
       <c r="F39" s="33"/>
       <c r="G39" s="22" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6466,29 +6480,27 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="60">
-    <mergeCell ref="F17:F18"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D34:D35"/>
+    <mergeCell ref="E34:E35"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
     <mergeCell ref="F34:F35"/>
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="F38:F39"/>
@@ -6505,27 +6517,29 @@
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="E17:E18"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="E34:E35"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F17:F18"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G4" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
@@ -6564,7 +6578,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.15">
       <c r="A1" s="23" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>0</v>
@@ -6573,7 +6587,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E1" s="15" t="s">
         <v>3</v>
@@ -6601,7 +6615,7 @@
         <v>19</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.15">
@@ -6609,10 +6623,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
@@ -6626,14 +6640,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
@@ -6643,10 +6657,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="16" t="s">
         <v>8</v>
@@ -6660,18 +6674,18 @@
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.15">
@@ -6679,10 +6693,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D7" s="16" t="s">
         <v>8</v>
@@ -6718,7 +6732,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D9" s="16" t="s">
         <v>8</v>
@@ -6736,12 +6750,12 @@
         <v>9</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C10" s="25"/>
       <c r="D10" s="25"/>
       <c r="E10" s="26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F10" s="25"/>
       <c r="G10" s="25"/>
@@ -6751,10 +6765,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D11" s="16" t="s">
         <v>8</v>
@@ -6766,22 +6780,22 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="80" x14ac:dyDescent="0.15">
-      <c r="A12" s="34">
+      <c r="A12" s="35">
         <v>11</v>
       </c>
-      <c r="B12" s="35" t="s">
-        <v>120</v>
+      <c r="B12" s="34" t="s">
+        <v>118</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D12" s="28"/>
       <c r="E12" s="28" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F12" s="32"/>
       <c r="G12" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.15">
@@ -6792,7 +6806,7 @@
       <c r="E13" s="30"/>
       <c r="F13" s="33"/>
       <c r="G13" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="48" x14ac:dyDescent="0.15">
@@ -6800,16 +6814,16 @@
         <v>12</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C14" s="26" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="26"/>
       <c r="F14" s="26"/>
       <c r="G14" s="26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="32" x14ac:dyDescent="0.15">
@@ -6817,10 +6831,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D15" s="16" t="s">
         <v>8</v>
@@ -6832,22 +6846,22 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="80" x14ac:dyDescent="0.15">
-      <c r="A16" s="34">
+      <c r="A16" s="35">
         <v>14</v>
       </c>
-      <c r="B16" s="35" t="s">
-        <v>125</v>
+      <c r="B16" s="34" t="s">
+        <v>123</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="28" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F16" s="32"/>
       <c r="G16" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.15">
@@ -6858,7 +6872,7 @@
       <c r="E17" s="30"/>
       <c r="F17" s="33"/>
       <c r="G17" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="48" x14ac:dyDescent="0.15">
@@ -6866,10 +6880,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C18" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>8</v>
@@ -6881,22 +6895,22 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="80" x14ac:dyDescent="0.15">
-      <c r="A19" s="34">
+      <c r="A19" s="35">
         <v>16</v>
       </c>
-      <c r="B19" s="35" t="s">
-        <v>128</v>
+      <c r="B19" s="34" t="s">
+        <v>126</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="28" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F19" s="32"/>
       <c r="G19" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.15">
@@ -6907,7 +6921,7 @@
       <c r="E20" s="30"/>
       <c r="F20" s="33"/>
       <c r="G20" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6915,10 +6929,10 @@
         <v>17</v>
       </c>
       <c r="B21" s="25" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D21" s="26" t="s">
         <v>8</v>
@@ -6934,10 +6948,10 @@
         <v>18</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C22" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D22" s="16" t="s">
         <v>8</v>
@@ -6949,22 +6963,22 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="34">
+      <c r="A23" s="35">
         <v>19</v>
       </c>
-      <c r="B23" s="35" t="s">
-        <v>131</v>
+      <c r="B23" s="34" t="s">
+        <v>129</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D23" s="28"/>
       <c r="E23" s="28" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F23" s="32"/>
       <c r="G23" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6975,7 +6989,7 @@
       <c r="E24" s="30"/>
       <c r="F24" s="33"/>
       <c r="G24" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -6983,10 +6997,10 @@
         <v>20</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D25" s="16" t="s">
         <v>8</v>
@@ -6996,22 +7010,22 @@
       <c r="G25" s="16"/>
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="34">
+      <c r="A26" s="35">
         <v>21</v>
       </c>
-      <c r="B26" s="35" t="s">
-        <v>134</v>
+      <c r="B26" s="34" t="s">
+        <v>132</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D26" s="28"/>
       <c r="E26" s="28" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F26" s="32"/>
       <c r="G26" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7022,7 +7036,7 @@
       <c r="E27" s="30"/>
       <c r="F27" s="33"/>
       <c r="G27" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7030,10 +7044,10 @@
         <v>22</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D28" s="16" t="s">
         <v>8</v>
@@ -7043,22 +7057,22 @@
       <c r="G28" s="16"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="34">
+      <c r="A29" s="35">
         <v>23</v>
       </c>
-      <c r="B29" s="35" t="s">
-        <v>137</v>
+      <c r="B29" s="34" t="s">
+        <v>135</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D29" s="28"/>
       <c r="E29" s="28" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F29" s="32"/>
       <c r="G29" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7069,7 +7083,7 @@
       <c r="E30" s="30"/>
       <c r="F30" s="33"/>
       <c r="G30" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7077,10 +7091,10 @@
         <v>24</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>8</v>
@@ -7090,22 +7104,22 @@
       <c r="G31" s="16"/>
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="34">
+      <c r="A32" s="35">
         <v>25</v>
       </c>
-      <c r="B32" s="35" t="s">
-        <v>140</v>
+      <c r="B32" s="34" t="s">
+        <v>138</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D32" s="28"/>
       <c r="E32" s="28" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F32" s="32"/>
       <c r="G32" s="17" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -7116,7 +7130,7 @@
       <c r="E33" s="30"/>
       <c r="F33" s="33"/>
       <c r="G33" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -15824,33 +15838,6 @@
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="F23:F24"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="F12:F13"/>
@@ -15866,6 +15853,33 @@
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="F29:F30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>

</xml_diff>